<commit_message>
Correctly formatting sort code, account number and invoice date columns
</commit_message>
<xml_diff>
--- a/assets/BulkSOP1 MOJ No Formatting.xlsx
+++ b/assets/BulkSOP1 MOJ No Formatting.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/refunds/opg-refunds-caseworker-api/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookPassword="93BE" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19420" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="34400" yWindow="460" windowWidth="34400" windowHeight="26740" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="3" state="hidden" r:id="rId1"/>
@@ -668,7 +668,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -705,6 +705,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -721,23 +723,7 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00EE6C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5B5B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1355,9 +1341,9 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AH302"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -1375,12 +1361,12 @@
     <col min="12" max="12" width="24.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.83203125" customWidth="1"/>
-    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.83203125" style="18" customWidth="1"/>
+    <col min="16" max="16" width="16" style="18" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.1640625" customWidth="1"/>
     <col min="18" max="18" width="19.1640625" customWidth="1"/>
-    <col min="19" max="19" width="17.33203125" customWidth="1"/>
-    <col min="20" max="20" width="14.6640625" customWidth="1"/>
+    <col min="19" max="19" width="17.33203125" style="18" customWidth="1"/>
+    <col min="20" max="20" width="14.6640625" style="19" customWidth="1"/>
     <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="23" max="28" width="11.5" bestFit="1" customWidth="1"/>
@@ -1436,10 +1422,10 @@
       <c r="N1" t="s">
         <v>73</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="19" t="s">
         <v>73</v>
       </c>
       <c r="U1" t="s">
@@ -1528,10 +1514,10 @@
       <c r="N2" t="s">
         <v>7</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="18" t="s">
         <v>9</v>
       </c>
       <c r="Q2" t="s">
@@ -1540,10 +1526,10 @@
       <c r="R2" t="s">
         <v>11</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="19" t="s">
         <v>13</v>
       </c>
       <c r="U2" t="s">

</xml_diff>